<commit_message>
all as of 23/05/2017
</commit_message>
<xml_diff>
--- a/data/meta.xlsx
+++ b/data/meta.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8078" windowHeight="1958" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8078" windowHeight="1958"/>
   </bookViews>
   <sheets>
     <sheet name="anobjl" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="trf" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">anobjl!$A$1:$C$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">anobjl!$A$1:$C$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">anobjw!$A$1:$F$46</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="135">
   <si>
     <t>object</t>
   </si>
@@ -133,15 +133,9 @@
     <t>wt</t>
   </si>
   <si>
-    <t>REPORT&gt;name|SEQUENCE</t>
-  </si>
-  <si>
     <t>SEQUENCE&gt;idx|GRAPH</t>
   </si>
   <si>
-    <t>STORAGE&gt;name|SEQUENCE</t>
-  </si>
-  <si>
     <t>SEQUENCE&gt;file|STORAGE</t>
   </si>
   <si>
@@ -226,12 +220,6 @@
     <t>GRAPH&gt;name</t>
   </si>
   <si>
-    <t>GRAPH&gt;id</t>
-  </si>
-  <si>
-    <t>SEQUENCE&gt;idx</t>
-  </si>
-  <si>
     <t>VERTEX&gt;membership2</t>
   </si>
   <si>
@@ -404,13 +392,46 @@
   </si>
   <si>
     <t>ENT_2&gt;id|OBS_2</t>
+  </si>
+  <si>
+    <t>VERTEX&gt;id|OBSERVATION</t>
+  </si>
+  <si>
+    <t>EDGE&gt;id|OBSERVATION</t>
+  </si>
+  <si>
+    <t>qa</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>gen</t>
+  </si>
+  <si>
+    <t>SEQUENCE&gt;step|GRAPH</t>
+  </si>
+  <si>
+    <t>SEQUENCE&gt;step</t>
+  </si>
+  <si>
+    <t>INFERENCE</t>
+  </si>
+  <si>
+    <t>SEQUENCE&gt;step|INFERENCE</t>
+  </si>
+  <si>
+    <t>INFERENCE&gt;id|OBSERVATION</t>
+  </si>
+  <si>
+    <t>tool_support</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,6 +441,21 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -447,13 +483,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -794,674 +838,708 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:C3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1328125" customWidth="1"/>
-    <col min="3" max="3" width="29.73046875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="32.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.1328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.73046875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="32.86328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
+      <c r="C2" s="7" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
+      <c r="C4" s="7" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
+      <c r="C5" s="7" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
+      <c r="C6" s="7" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="B12" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="B13" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="B49" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" s="7">
         <v>2</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="7">
         <v>2</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C58" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A59" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A60" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>33</v>
-      </c>
-      <c r="B43" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+      <c r="B60" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A61" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B47" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>45</v>
-      </c>
-      <c r="B48" t="s">
-        <v>36</v>
-      </c>
-      <c r="C48" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49" t="s">
-        <v>36</v>
-      </c>
-      <c r="C49" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>46</v>
-      </c>
-      <c r="B50" t="s">
-        <v>36</v>
-      </c>
-      <c r="C50" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>70</v>
-      </c>
-      <c r="B51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C51" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
-        <v>44</v>
-      </c>
-      <c r="B52" t="s">
-        <v>36</v>
-      </c>
-      <c r="C52" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" t="s">
-        <v>36</v>
-      </c>
-      <c r="C53" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
-        <v>47</v>
-      </c>
-      <c r="B54" t="s">
-        <v>36</v>
-      </c>
-      <c r="C54" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>48</v>
-      </c>
-      <c r="B55" t="s">
-        <v>36</v>
-      </c>
-      <c r="C55" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>49</v>
-      </c>
-      <c r="B56" t="s">
-        <v>36</v>
-      </c>
-      <c r="C56" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>52</v>
-      </c>
-      <c r="B57" t="s">
-        <v>36</v>
-      </c>
-      <c r="C57" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" t="s">
-        <v>36</v>
-      </c>
-      <c r="C58" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>69</v>
-      </c>
-      <c r="B59" t="s">
-        <v>36</v>
-      </c>
-      <c r="C59" s="3">
+      <c r="B61" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A62" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C62" s="7">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C58"/>
-  <sortState ref="A2:C11">
-    <sortCondition ref="A2:A11"/>
+  <autoFilter ref="A1:C61"/>
+  <sortState ref="A2:C16">
+    <sortCondition ref="A2:A16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1491,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>17</v>
@@ -1511,7 +1589,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -1522,10 +1600,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1533,10 +1611,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F4">
         <v>6</v>
@@ -1544,10 +1622,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -1555,10 +1633,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -1566,10 +1644,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -1580,7 +1658,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -1591,10 +1669,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -1605,7 +1683,7 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -1616,7 +1694,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F11">
         <v>6</v>
@@ -1627,7 +1705,7 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -1638,7 +1716,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -1649,7 +1727,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F14">
         <v>6</v>
@@ -1660,7 +1738,7 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -1668,10 +1746,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -1682,7 +1760,7 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -1693,7 +1771,7 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F18">
         <v>6</v>
@@ -1704,7 +1782,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F19">
         <v>3</v>
@@ -1715,7 +1793,7 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F20">
         <v>3</v>
@@ -1723,10 +1801,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F21">
         <v>3</v>
@@ -1737,7 +1815,7 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F22">
         <v>3</v>
@@ -1745,10 +1823,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F23">
         <v>3</v>
@@ -1759,7 +1837,7 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -1770,7 +1848,7 @@
         <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -1781,7 +1859,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F26">
         <v>6</v>
@@ -1792,7 +1870,7 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
@@ -1806,7 +1884,7 @@
         <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F28">
         <v>3</v>
@@ -1817,7 +1895,7 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
         <v>20</v>
@@ -1831,7 +1909,7 @@
         <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E30" t="s">
         <v>18</v>
@@ -1845,7 +1923,7 @@
         <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F31">
         <v>6</v>
@@ -1856,7 +1934,7 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
@@ -1867,10 +1945,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -1881,7 +1959,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
@@ -1892,10 +1970,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
@@ -1903,10 +1981,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -1917,7 +1995,7 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -1928,10 +2006,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
@@ -1942,7 +2020,7 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
@@ -1953,10 +2031,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F40">
         <v>3</v>
@@ -1964,10 +2042,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F41">
         <v>3</v>
@@ -1975,10 +2053,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F42">
         <v>6</v>
@@ -1986,10 +2064,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F43">
         <v>6</v>
@@ -1997,10 +2075,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F44">
         <v>3</v>
@@ -2008,10 +2086,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F45">
         <v>6</v>
@@ -2019,10 +2097,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F46">
         <v>3</v>
@@ -2039,8 +2117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2062,40 +2140,40 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -2106,7 +2184,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -2117,7 +2195,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -2128,29 +2206,29 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -2161,7 +2239,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -2172,7 +2250,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
@@ -2183,7 +2261,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
@@ -2194,7 +2272,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
         <v>36</v>
@@ -2205,7 +2283,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
         <v>36</v>
@@ -2216,7 +2294,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
         <v>36</v>
@@ -2227,7 +2305,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -2238,7 +2316,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -2249,7 +2327,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B19" t="s">
         <v>36</v>
@@ -2260,7 +2338,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
@@ -2271,7 +2349,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
@@ -2282,7 +2360,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
@@ -2293,7 +2371,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
@@ -2304,7 +2382,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
@@ -2315,7 +2393,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
@@ -2326,7 +2404,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B26" t="s">
         <v>19</v>
@@ -2337,7 +2415,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B27" t="s">
         <v>19</v>
@@ -2348,7 +2426,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
         <v>19</v>
@@ -2359,7 +2437,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
         <v>19</v>
@@ -2370,7 +2448,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
         <v>19</v>
@@ -2381,7 +2459,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
         <v>19</v>
@@ -2392,7 +2470,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
         <v>19</v>
@@ -2403,7 +2481,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
         <v>19</v>
@@ -2414,7 +2492,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
         <v>19</v>
@@ -2425,7 +2503,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
         <v>19</v>
@@ -2436,7 +2514,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
         <v>36</v>
@@ -2447,7 +2525,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
@@ -2458,7 +2536,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
@@ -2469,7 +2547,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
         <v>36</v>
@@ -2480,7 +2558,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B40" t="s">
         <v>36</v>
@@ -2491,7 +2569,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B41" t="s">
         <v>36</v>
@@ -2502,7 +2580,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B42" t="s">
         <v>19</v>
@@ -2513,7 +2591,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
         <v>19</v>
@@ -2524,7 +2602,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B44" t="s">
         <v>19</v>
@@ -2535,7 +2613,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
@@ -2546,7 +2624,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
         <v>19</v>
@@ -2557,7 +2635,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
@@ -2568,7 +2646,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B48" t="s">
         <v>19</v>
@@ -2579,7 +2657,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B49" t="s">
         <v>19</v>
@@ -2590,7 +2668,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B50" t="s">
         <v>19</v>
@@ -2601,7 +2679,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B51" t="s">
         <v>19</v>
@@ -2612,7 +2690,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B52" t="s">
         <v>19</v>
@@ -2623,7 +2701,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B53" t="s">
         <v>19</v>
@@ -2634,7 +2712,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B54" t="s">
         <v>19</v>
@@ -2645,7 +2723,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
         <v>36</v>
@@ -2656,7 +2734,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B56" t="s">
         <v>36</v>
@@ -2667,7 +2745,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B57" t="s">
         <v>36</v>
@@ -2678,7 +2756,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B58" t="s">
         <v>36</v>
@@ -2689,7 +2767,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B59" t="s">
         <v>36</v>
@@ -2700,7 +2778,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
working on product reverse engineering example
</commit_message>
<xml_diff>
--- a/data/meta.xlsx
+++ b/data/meta.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8078" windowHeight="1958"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8085" windowHeight="1965"/>
   </bookViews>
   <sheets>
     <sheet name="anobjl" sheetId="1" r:id="rId1"/>
@@ -841,20 +841,20 @@
   <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.1328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.73046875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="32.86328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="6"/>
+    <col min="3" max="3" width="29.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -865,73 +865,73 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>131</v>
+        <v>9</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>9</v>
+        <v>131</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -942,7 +942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>5</v>
       </c>
@@ -953,7 +953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>3</v>
       </c>
@@ -964,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>131</v>
       </c>
@@ -975,7 +975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
@@ -986,7 +986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
@@ -997,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>124</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>125</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>129</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>132</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>34</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>35</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>133</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>13</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>3</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>131</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>10</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>9</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>13</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>12</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>14</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>15</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>65</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>21</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>61</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>64</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>63</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>25</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>62</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>27</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>48</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>29</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>49</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>30</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>31</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>32</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>33</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>40</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>41</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>51</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>43</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>67</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>44</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>66</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>42</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>52</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>45</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>46</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>47</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>50</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>53</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>130</v>
       </c>
@@ -1538,8 +1538,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C61"/>
-  <sortState ref="A2:C16">
-    <sortCondition ref="A2:A16"/>
+  <sortState ref="A3:C16">
+    <sortCondition ref="A3:A16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1555,16 +1555,16 @@
       <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.73046875" customWidth="1"/>
-    <col min="4" max="4" width="7.3984375" customWidth="1"/>
-    <col min="5" max="5" width="25.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>59</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -2121,13 +2121,13 @@
       <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>114</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>120</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>113</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>114</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>116</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>121</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>108</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>109</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>110</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>100</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>99</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>101</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>102</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>107</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>92</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>89</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>90</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>95</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>71</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>73</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>74</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>75</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>77</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>79</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>80</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>81</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>88</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>83</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>84</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>85</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>86</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>87</v>
       </c>

</xml_diff>